<commit_message>
did the initial evaluation, started testing another configuration for the no edges no weighted mean
</commit_message>
<xml_diff>
--- a/project/code/model_checkpoints/configurations.xlsx
+++ b/project/code/model_checkpoints/configurations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\instance-seg\project\code\model_checkpoints\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{038786DE-A23F-4DFB-98B2-BD7C3D973A04}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D4EAE20-F6EC-4EDF-8EFE-0DEB0E9A2936}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1130" uniqueCount="27">
   <si>
     <t>alpha</t>
   </si>
@@ -53,12 +53,66 @@
   <si>
     <t>V</t>
   </si>
+  <si>
+    <t>SBD</t>
+  </si>
+  <si>
+    <t>FBD</t>
+  </si>
+  <si>
+    <t>DiC</t>
+  </si>
+  <si>
+    <t>without edges without weighted mean</t>
+  </si>
+  <si>
+    <t>without edges with weighted mean</t>
+  </si>
+  <si>
+    <t>with edges without weighted mean</t>
+  </si>
+  <si>
+    <t>with edges with weighted mean</t>
+  </si>
+  <si>
+    <t>Initial results - HDBSCAN only</t>
+  </si>
+  <si>
+    <t>original paper</t>
+  </si>
+  <si>
+    <t>500 epochs</t>
+  </si>
+  <si>
+    <t>1000 epochs</t>
+  </si>
+  <si>
+    <t>HDBSCAN only</t>
+  </si>
+  <si>
+    <t>HDBSCAN+MRF</t>
+  </si>
+  <si>
+    <t>HDBSCAN+clusternet</t>
+  </si>
+  <si>
+    <t>HDBSCAN+MRF+clusternet</t>
+  </si>
+  <si>
+    <t>HDBSCAN+clusternet+MRF</t>
+  </si>
+  <si>
+    <t>HDBSCAN+MRF+clusternet+MRF</t>
+  </si>
+  <si>
+    <t>Best full evaluation</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -74,16 +128,49 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -91,16 +178,43 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Output" xfId="1" builtinId="21"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -378,19 +492,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F49"/>
+  <dimension ref="A1:AH49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="F49" sqref="F49"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="X24" sqref="X24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="7.375" customWidth="1"/>
     <col min="5" max="5" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="29.5" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="29.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -409,8 +526,34 @@
       <c r="F1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="Z1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA1" s="2"/>
+      <c r="AB1" s="2"/>
+      <c r="AC1" s="2"/>
+      <c r="AD1" s="2"/>
+      <c r="AE1" s="2"/>
+      <c r="AF1" s="2"/>
+      <c r="AG1" s="2"/>
+      <c r="AH1" s="2"/>
+    </row>
+    <row r="2" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -426,11 +569,33 @@
       <c r="E2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="Z2" s="2"/>
+      <c r="AA2" s="2"/>
+      <c r="AB2" s="2"/>
+      <c r="AC2" s="2"/>
+      <c r="AD2" s="2"/>
+      <c r="AE2" s="2"/>
+      <c r="AF2" s="2"/>
+      <c r="AG2" s="2"/>
+      <c r="AH2" s="2"/>
+    </row>
+    <row r="3" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -446,11 +611,41 @@
       <c r="E3" t="s">
         <v>6</v>
       </c>
-      <c r="F3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+      <c r="Z3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA3" s="2"/>
+      <c r="AB3" s="2"/>
+      <c r="AC3" s="2"/>
+      <c r="AD3" s="9"/>
+      <c r="AE3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AF3" s="2"/>
+      <c r="AG3" s="2"/>
+      <c r="AH3" s="2"/>
+    </row>
+    <row r="4" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -466,11 +661,69 @@
       <c r="E4" t="s">
         <v>5</v>
       </c>
-      <c r="F4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="T4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="AC4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD4" s="3"/>
+      <c r="AE4" s="3"/>
+      <c r="AF4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AG4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="AH4" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -486,11 +739,61 @@
       <c r="E5" t="s">
         <v>6</v>
       </c>
-      <c r="F5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" s="6">
+        <v>1</v>
+      </c>
+      <c r="I5" s="6">
+        <v>5</v>
+      </c>
+      <c r="J5" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="K5" s="6">
+        <v>0.3609</v>
+      </c>
+      <c r="L5" s="6">
+        <v>0.78839999999999999</v>
+      </c>
+      <c r="M5" s="6">
+        <v>21</v>
+      </c>
+      <c r="N5" s="3"/>
+      <c r="O5" s="6">
+        <v>1</v>
+      </c>
+      <c r="P5" s="6">
+        <v>5</v>
+      </c>
+      <c r="Q5" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="R5" s="6">
+        <v>0.36249999999999999</v>
+      </c>
+      <c r="S5" s="6">
+        <v>0.77339999999999998</v>
+      </c>
+      <c r="T5" s="6">
+        <v>22.95</v>
+      </c>
+      <c r="Z5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA5" s="3"/>
+      <c r="AB5" s="3"/>
+      <c r="AC5" s="3"/>
+      <c r="AD5" s="3"/>
+      <c r="AE5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="AF5" s="3"/>
+      <c r="AG5" s="3"/>
+      <c r="AH5" s="3"/>
+    </row>
+    <row r="6" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -506,11 +809,61 @@
       <c r="E6" t="s">
         <v>5</v>
       </c>
-      <c r="F6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="6">
+        <v>1</v>
+      </c>
+      <c r="I6" s="6">
+        <v>5</v>
+      </c>
+      <c r="J6" s="6">
+        <v>1</v>
+      </c>
+      <c r="K6" s="6">
+        <v>0.38440000000000002</v>
+      </c>
+      <c r="L6" s="6">
+        <v>0.76619999999999999</v>
+      </c>
+      <c r="M6" s="6">
+        <v>21.75</v>
+      </c>
+      <c r="N6" s="3"/>
+      <c r="O6" s="6">
+        <v>1</v>
+      </c>
+      <c r="P6" s="6">
+        <v>5</v>
+      </c>
+      <c r="Q6" s="6">
+        <v>1</v>
+      </c>
+      <c r="R6" s="6">
+        <v>0.40820000000000001</v>
+      </c>
+      <c r="S6" s="6">
+        <v>0.79769999999999996</v>
+      </c>
+      <c r="T6" s="6">
+        <v>17.25</v>
+      </c>
+      <c r="Z6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA6" s="3"/>
+      <c r="AB6" s="3"/>
+      <c r="AC6" s="3"/>
+      <c r="AD6" s="3"/>
+      <c r="AE6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="AF6" s="3"/>
+      <c r="AG6" s="3"/>
+      <c r="AH6" s="3"/>
+    </row>
+    <row r="7" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -526,11 +879,61 @@
       <c r="E7" t="s">
         <v>6</v>
       </c>
-      <c r="F7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" s="6">
+        <v>1</v>
+      </c>
+      <c r="I7" s="6">
+        <v>10</v>
+      </c>
+      <c r="J7" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="K7" s="6">
+        <v>0.42459999999999998</v>
+      </c>
+      <c r="L7" s="6">
+        <v>0.79820000000000002</v>
+      </c>
+      <c r="M7" s="6">
+        <v>18.7</v>
+      </c>
+      <c r="N7" s="3"/>
+      <c r="O7" s="6">
+        <v>1</v>
+      </c>
+      <c r="P7" s="6">
+        <v>10</v>
+      </c>
+      <c r="Q7" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="R7" s="6">
+        <v>0.42030000000000001</v>
+      </c>
+      <c r="S7" s="6">
+        <v>0.80630000000000002</v>
+      </c>
+      <c r="T7" s="6">
+        <v>16.55</v>
+      </c>
+      <c r="Z7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="AA7" s="3"/>
+      <c r="AB7" s="3"/>
+      <c r="AC7" s="3"/>
+      <c r="AD7" s="3"/>
+      <c r="AE7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="AF7" s="3"/>
+      <c r="AG7" s="3"/>
+      <c r="AH7" s="3"/>
+    </row>
+    <row r="8" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
@@ -546,8 +949,59 @@
       <c r="E8" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F8" s="5"/>
+      <c r="H8" s="6">
+        <v>1</v>
+      </c>
+      <c r="I8" s="6">
+        <v>10</v>
+      </c>
+      <c r="J8" s="6">
+        <v>1</v>
+      </c>
+      <c r="K8" s="6">
+        <v>0.45660000000000001</v>
+      </c>
+      <c r="L8" s="6">
+        <v>0.83899999999999997</v>
+      </c>
+      <c r="M8" s="6">
+        <v>14.05</v>
+      </c>
+      <c r="N8" s="3"/>
+      <c r="O8" s="6">
+        <v>1</v>
+      </c>
+      <c r="P8" s="6">
+        <v>10</v>
+      </c>
+      <c r="Q8" s="6">
+        <v>1</v>
+      </c>
+      <c r="R8" s="6">
+        <v>0.45750000000000002</v>
+      </c>
+      <c r="S8" s="6">
+        <v>0.82730000000000004</v>
+      </c>
+      <c r="T8" s="6">
+        <v>14.55</v>
+      </c>
+      <c r="Z8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA8" s="3"/>
+      <c r="AB8" s="3"/>
+      <c r="AC8" s="3"/>
+      <c r="AD8" s="3"/>
+      <c r="AE8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF8" s="3"/>
+      <c r="AG8" s="3"/>
+      <c r="AH8" s="3"/>
+    </row>
+    <row r="9" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
@@ -563,8 +1017,59 @@
       <c r="E9" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F9" s="5"/>
+      <c r="H9" s="7">
+        <v>1</v>
+      </c>
+      <c r="I9" s="7">
+        <v>20</v>
+      </c>
+      <c r="J9" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="K9" s="7">
+        <v>0.54569999999999996</v>
+      </c>
+      <c r="L9" s="7">
+        <v>0.85019999999999996</v>
+      </c>
+      <c r="M9" s="7">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="N9" s="3"/>
+      <c r="O9" s="6">
+        <v>1</v>
+      </c>
+      <c r="P9" s="6">
+        <v>20</v>
+      </c>
+      <c r="Q9" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="R9" s="6">
+        <v>0.45429999999999998</v>
+      </c>
+      <c r="S9" s="6">
+        <v>0.74390000000000001</v>
+      </c>
+      <c r="T9" s="6">
+        <v>16.7</v>
+      </c>
+      <c r="Z9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA9" s="3"/>
+      <c r="AB9" s="3"/>
+      <c r="AC9" s="3"/>
+      <c r="AD9" s="3"/>
+      <c r="AE9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="AF9" s="3"/>
+      <c r="AG9" s="3"/>
+      <c r="AH9" s="3"/>
+    </row>
+    <row r="10" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
@@ -580,11 +1085,61 @@
       <c r="E10" t="s">
         <v>5</v>
       </c>
-      <c r="F10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10" s="7">
+        <v>1</v>
+      </c>
+      <c r="I10" s="7">
+        <v>20</v>
+      </c>
+      <c r="J10" s="7">
+        <v>1</v>
+      </c>
+      <c r="K10" s="7">
+        <v>0.52710000000000001</v>
+      </c>
+      <c r="L10" s="7">
+        <v>0.88780000000000003</v>
+      </c>
+      <c r="M10" s="7">
+        <v>11</v>
+      </c>
+      <c r="N10" s="3"/>
+      <c r="O10" s="7">
+        <v>1</v>
+      </c>
+      <c r="P10" s="7">
+        <v>20</v>
+      </c>
+      <c r="Q10" s="7">
+        <v>1</v>
+      </c>
+      <c r="R10" s="7">
+        <v>0.50139999999999996</v>
+      </c>
+      <c r="S10" s="7">
+        <v>0.79239999999999999</v>
+      </c>
+      <c r="T10" s="7">
+        <v>11.65</v>
+      </c>
+      <c r="Z10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA10" s="3"/>
+      <c r="AB10" s="3"/>
+      <c r="AC10" s="3"/>
+      <c r="AD10" s="3"/>
+      <c r="AE10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="AF10" s="3"/>
+      <c r="AG10" s="3"/>
+      <c r="AH10" s="3"/>
+    </row>
+    <row r="11" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
@@ -600,11 +1155,45 @@
       <c r="E11" t="s">
         <v>6</v>
       </c>
-      <c r="F11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F11" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H11" s="7">
+        <v>1</v>
+      </c>
+      <c r="I11" s="7">
+        <v>20</v>
+      </c>
+      <c r="J11" s="7">
+        <v>2</v>
+      </c>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="7">
+        <v>1</v>
+      </c>
+      <c r="P11" s="7">
+        <v>20</v>
+      </c>
+      <c r="Q11" s="7">
+        <v>2</v>
+      </c>
+      <c r="R11" s="7"/>
+      <c r="S11" s="7"/>
+      <c r="T11" s="7"/>
+      <c r="Z11" s="3"/>
+      <c r="AA11" s="3"/>
+      <c r="AB11" s="3"/>
+      <c r="AC11" s="3"/>
+      <c r="AD11" s="3"/>
+      <c r="AE11" s="3"/>
+      <c r="AF11" s="3"/>
+      <c r="AG11" s="3"/>
+      <c r="AH11" s="3"/>
+    </row>
+    <row r="12" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
@@ -620,11 +1209,57 @@
       <c r="E12" t="s">
         <v>5</v>
       </c>
-      <c r="F12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F12" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H12" s="6">
+        <v>2</v>
+      </c>
+      <c r="I12" s="6">
+        <v>5</v>
+      </c>
+      <c r="J12" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="K12" s="6">
+        <v>0.3931</v>
+      </c>
+      <c r="L12" s="6">
+        <v>0.75480000000000003</v>
+      </c>
+      <c r="M12" s="6">
+        <v>24.85</v>
+      </c>
+      <c r="N12" s="3"/>
+      <c r="O12" s="6">
+        <v>2</v>
+      </c>
+      <c r="P12" s="6">
+        <v>5</v>
+      </c>
+      <c r="Q12" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="R12" s="6">
+        <v>0.42849999999999999</v>
+      </c>
+      <c r="S12" s="6">
+        <v>0.82211999999999996</v>
+      </c>
+      <c r="T12" s="6">
+        <v>18.7</v>
+      </c>
+      <c r="Z12" s="3"/>
+      <c r="AA12" s="3"/>
+      <c r="AB12" s="3"/>
+      <c r="AC12" s="3"/>
+      <c r="AD12" s="3"/>
+      <c r="AE12" s="3"/>
+      <c r="AF12" s="3"/>
+      <c r="AG12" s="3"/>
+      <c r="AH12" s="3"/>
+    </row>
+    <row r="13" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
       </c>
@@ -640,11 +1275,61 @@
       <c r="E13" t="s">
         <v>6</v>
       </c>
-      <c r="F13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F13" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H13" s="6">
+        <v>2</v>
+      </c>
+      <c r="I13" s="6">
+        <v>5</v>
+      </c>
+      <c r="J13" s="6">
+        <v>1</v>
+      </c>
+      <c r="K13" s="6">
+        <v>0.42799999999999999</v>
+      </c>
+      <c r="L13" s="6">
+        <v>0.7984</v>
+      </c>
+      <c r="M13" s="6">
+        <v>13.7</v>
+      </c>
+      <c r="N13" s="3"/>
+      <c r="O13" s="6">
+        <v>2</v>
+      </c>
+      <c r="P13" s="6">
+        <v>5</v>
+      </c>
+      <c r="Q13" s="6">
+        <v>1</v>
+      </c>
+      <c r="R13" s="6">
+        <v>0.39900000000000002</v>
+      </c>
+      <c r="S13" s="6">
+        <v>0.81</v>
+      </c>
+      <c r="T13" s="6">
+        <v>19.8</v>
+      </c>
+      <c r="Z13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA13" s="2"/>
+      <c r="AB13" s="2"/>
+      <c r="AC13" s="2"/>
+      <c r="AD13" s="9"/>
+      <c r="AE13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AF13" s="2"/>
+      <c r="AG13" s="2"/>
+      <c r="AH13" s="2"/>
+    </row>
+    <row r="14" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1</v>
       </c>
@@ -660,11 +1345,69 @@
       <c r="E14" t="s">
         <v>5</v>
       </c>
-      <c r="F14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F14" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H14" s="6">
+        <v>2</v>
+      </c>
+      <c r="I14" s="6">
+        <v>10</v>
+      </c>
+      <c r="J14" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="K14" s="6">
+        <v>0.46350000000000002</v>
+      </c>
+      <c r="L14" s="6">
+        <v>0.82650000000000001</v>
+      </c>
+      <c r="M14" s="6">
+        <v>13.4</v>
+      </c>
+      <c r="N14" s="3"/>
+      <c r="O14" s="6">
+        <v>2</v>
+      </c>
+      <c r="P14" s="6">
+        <v>10</v>
+      </c>
+      <c r="Q14" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="R14" s="6">
+        <v>0.26390000000000002</v>
+      </c>
+      <c r="S14" s="6">
+        <v>0.53249999999999997</v>
+      </c>
+      <c r="T14" s="6">
+        <v>43.25</v>
+      </c>
+      <c r="Z14" s="3"/>
+      <c r="AA14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="AC14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD14" s="3"/>
+      <c r="AE14" s="3"/>
+      <c r="AF14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AG14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="AH14" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1</v>
       </c>
@@ -680,11 +1423,61 @@
       <c r="E15" t="s">
         <v>6</v>
       </c>
-      <c r="F15" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F15" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H15" s="6">
+        <v>2</v>
+      </c>
+      <c r="I15" s="6">
+        <v>10</v>
+      </c>
+      <c r="J15" s="6">
+        <v>1</v>
+      </c>
+      <c r="K15" s="6">
+        <v>0.4481</v>
+      </c>
+      <c r="L15" s="6">
+        <v>0.85150000000000003</v>
+      </c>
+      <c r="M15" s="6">
+        <v>15.1</v>
+      </c>
+      <c r="N15" s="3"/>
+      <c r="O15" s="6">
+        <v>2</v>
+      </c>
+      <c r="P15" s="6">
+        <v>10</v>
+      </c>
+      <c r="Q15" s="6">
+        <v>1</v>
+      </c>
+      <c r="R15" s="6">
+        <v>0.44600000000000001</v>
+      </c>
+      <c r="S15" s="6">
+        <v>0.82769999999999999</v>
+      </c>
+      <c r="T15" s="6">
+        <v>14.45</v>
+      </c>
+      <c r="Z15" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA15" s="3"/>
+      <c r="AB15" s="3"/>
+      <c r="AC15" s="3"/>
+      <c r="AD15" s="3"/>
+      <c r="AE15" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="AF15" s="3"/>
+      <c r="AG15" s="3"/>
+      <c r="AH15" s="3"/>
+    </row>
+    <row r="16" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1</v>
       </c>
@@ -700,8 +1493,59 @@
       <c r="E16" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F16" s="5"/>
+      <c r="H16" s="6">
+        <v>2</v>
+      </c>
+      <c r="I16" s="6">
+        <v>20</v>
+      </c>
+      <c r="J16" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="K16" s="6">
+        <v>0.27289999999999998</v>
+      </c>
+      <c r="L16" s="6">
+        <v>0.67449999999999999</v>
+      </c>
+      <c r="M16" s="6">
+        <v>75.650000000000006</v>
+      </c>
+      <c r="N16" s="3"/>
+      <c r="O16" s="6">
+        <v>2</v>
+      </c>
+      <c r="P16" s="6">
+        <v>20</v>
+      </c>
+      <c r="Q16" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="R16" s="6">
+        <v>0.4965</v>
+      </c>
+      <c r="S16" s="6">
+        <v>0.83350000000000002</v>
+      </c>
+      <c r="T16" s="6">
+        <v>16.75</v>
+      </c>
+      <c r="Z16" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA16" s="3"/>
+      <c r="AB16" s="3"/>
+      <c r="AC16" s="3"/>
+      <c r="AD16" s="3"/>
+      <c r="AE16" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="AF16" s="3"/>
+      <c r="AG16" s="3"/>
+      <c r="AH16" s="3"/>
+    </row>
+    <row r="17" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1</v>
       </c>
@@ -717,8 +1561,47 @@
       <c r="E17" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F17" s="5"/>
+      <c r="H17" s="6">
+        <v>2</v>
+      </c>
+      <c r="I17" s="6">
+        <v>20</v>
+      </c>
+      <c r="J17" s="6">
+        <v>1</v>
+      </c>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="6">
+        <v>2</v>
+      </c>
+      <c r="P17" s="6">
+        <v>20</v>
+      </c>
+      <c r="Q17" s="6">
+        <v>1</v>
+      </c>
+      <c r="R17" s="6"/>
+      <c r="S17" s="6"/>
+      <c r="T17" s="6"/>
+      <c r="Z17" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="AA17" s="3"/>
+      <c r="AB17" s="3"/>
+      <c r="AC17" s="3"/>
+      <c r="AD17" s="3"/>
+      <c r="AE17" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="AF17" s="3"/>
+      <c r="AG17" s="3"/>
+      <c r="AH17" s="3"/>
+    </row>
+    <row r="18" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1</v>
       </c>
@@ -734,11 +1617,49 @@
       <c r="E18" t="s">
         <v>5</v>
       </c>
-      <c r="F18" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F18" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H18" s="6">
+        <v>2</v>
+      </c>
+      <c r="I18" s="6">
+        <v>20</v>
+      </c>
+      <c r="J18" s="6">
+        <v>2</v>
+      </c>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="6">
+        <v>2</v>
+      </c>
+      <c r="P18" s="6">
+        <v>20</v>
+      </c>
+      <c r="Q18" s="6">
+        <v>2</v>
+      </c>
+      <c r="R18" s="6"/>
+      <c r="S18" s="6"/>
+      <c r="T18" s="6"/>
+      <c r="Z18" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA18" s="3"/>
+      <c r="AB18" s="3"/>
+      <c r="AC18" s="3"/>
+      <c r="AD18" s="3"/>
+      <c r="AE18" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF18" s="3"/>
+      <c r="AG18" s="3"/>
+      <c r="AH18" s="3"/>
+    </row>
+    <row r="19" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1</v>
       </c>
@@ -754,11 +1675,41 @@
       <c r="E19" t="s">
         <v>6</v>
       </c>
-      <c r="F19" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F19" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="P19" s="2"/>
+      <c r="Q19" s="2"/>
+      <c r="R19" s="2"/>
+      <c r="S19" s="2"/>
+      <c r="T19" s="2"/>
+      <c r="Z19" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA19" s="3"/>
+      <c r="AB19" s="3"/>
+      <c r="AC19" s="3"/>
+      <c r="AD19" s="3"/>
+      <c r="AE19" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="AF19" s="3"/>
+      <c r="AG19" s="3"/>
+      <c r="AH19" s="3"/>
+    </row>
+    <row r="20" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1</v>
       </c>
@@ -774,8 +1725,61 @@
       <c r="E20" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F20" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L20" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="M20" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="P20" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="R20" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="S20" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="T20" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z20" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA20" s="3"/>
+      <c r="AB20" s="3"/>
+      <c r="AC20" s="3"/>
+      <c r="AD20" s="3"/>
+      <c r="AE20" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="AF20" s="3"/>
+      <c r="AG20" s="3"/>
+      <c r="AH20" s="3"/>
+    </row>
+    <row r="21" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1</v>
       </c>
@@ -791,11 +1795,57 @@
       <c r="E21" t="s">
         <v>6</v>
       </c>
-      <c r="F21" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F21" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H21" s="6">
+        <v>1</v>
+      </c>
+      <c r="I21" s="6">
+        <v>5</v>
+      </c>
+      <c r="J21" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="K21" s="6">
+        <v>0.31609999999999999</v>
+      </c>
+      <c r="L21" s="6">
+        <v>0.63670000000000004</v>
+      </c>
+      <c r="M21" s="6">
+        <v>24.15</v>
+      </c>
+      <c r="N21" s="3"/>
+      <c r="O21" s="7">
+        <v>1</v>
+      </c>
+      <c r="P21" s="7">
+        <v>5</v>
+      </c>
+      <c r="Q21" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="R21" s="7">
+        <v>0.35659999999999997</v>
+      </c>
+      <c r="S21" s="7">
+        <v>0.72709999999999997</v>
+      </c>
+      <c r="T21" s="7">
+        <v>21.7</v>
+      </c>
+      <c r="Z21" s="3"/>
+      <c r="AA21" s="3"/>
+      <c r="AB21" s="3"/>
+      <c r="AC21" s="3"/>
+      <c r="AD21" s="3"/>
+      <c r="AE21" s="3"/>
+      <c r="AF21" s="3"/>
+      <c r="AG21" s="3"/>
+      <c r="AH21" s="3"/>
+    </row>
+    <row r="22" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1</v>
       </c>
@@ -811,11 +1861,45 @@
       <c r="E22" t="s">
         <v>5</v>
       </c>
-      <c r="F22" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F22" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H22" s="6">
+        <v>1</v>
+      </c>
+      <c r="I22" s="6">
+        <v>5</v>
+      </c>
+      <c r="J22" s="6">
+        <v>1</v>
+      </c>
+      <c r="K22" s="8"/>
+      <c r="L22" s="8"/>
+      <c r="M22" s="8"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="6">
+        <v>1</v>
+      </c>
+      <c r="P22" s="6">
+        <v>5</v>
+      </c>
+      <c r="Q22" s="6">
+        <v>1</v>
+      </c>
+      <c r="R22" s="6"/>
+      <c r="S22" s="6"/>
+      <c r="T22" s="6"/>
+      <c r="Z22" s="3"/>
+      <c r="AA22" s="3"/>
+      <c r="AB22" s="3"/>
+      <c r="AC22" s="3"/>
+      <c r="AD22" s="3"/>
+      <c r="AE22" s="3"/>
+      <c r="AF22" s="3"/>
+      <c r="AG22" s="3"/>
+      <c r="AH22" s="3"/>
+    </row>
+    <row r="23" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1</v>
       </c>
@@ -831,11 +1915,59 @@
       <c r="E23" t="s">
         <v>6</v>
       </c>
-      <c r="F23" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F23" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H23" s="7">
+        <v>1</v>
+      </c>
+      <c r="I23" s="7">
+        <v>10</v>
+      </c>
+      <c r="J23" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="K23" s="7">
+        <v>0.38200000000000001</v>
+      </c>
+      <c r="L23" s="7">
+        <v>0.71789999999999998</v>
+      </c>
+      <c r="M23" s="7">
+        <v>20.2</v>
+      </c>
+      <c r="N23" s="3"/>
+      <c r="O23" s="6">
+        <v>1</v>
+      </c>
+      <c r="P23" s="6">
+        <v>10</v>
+      </c>
+      <c r="Q23" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="R23" s="6">
+        <v>0.27910000000000001</v>
+      </c>
+      <c r="S23" s="6">
+        <v>0.58289999999999997</v>
+      </c>
+      <c r="T23" s="6">
+        <v>34.200000000000003</v>
+      </c>
+      <c r="Z23" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA23" s="2"/>
+      <c r="AB23" s="2"/>
+      <c r="AC23" s="2"/>
+      <c r="AD23" s="3"/>
+      <c r="AE23" s="3"/>
+      <c r="AF23" s="3"/>
+      <c r="AG23" s="3"/>
+      <c r="AH23" s="3"/>
+    </row>
+    <row r="24" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1</v>
       </c>
@@ -851,8 +1983,49 @@
       <c r="E24" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F24" s="5"/>
+      <c r="H24" s="6">
+        <v>1</v>
+      </c>
+      <c r="I24" s="6">
+        <v>10</v>
+      </c>
+      <c r="J24" s="6">
+        <v>1</v>
+      </c>
+      <c r="K24" s="6"/>
+      <c r="L24" s="6"/>
+      <c r="M24" s="6"/>
+      <c r="N24" s="3"/>
+      <c r="O24" s="6">
+        <v>1</v>
+      </c>
+      <c r="P24" s="6">
+        <v>10</v>
+      </c>
+      <c r="Q24" s="6">
+        <v>1</v>
+      </c>
+      <c r="R24" s="6"/>
+      <c r="S24" s="6"/>
+      <c r="T24" s="6"/>
+      <c r="Z24" s="3"/>
+      <c r="AA24" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB24" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="AC24" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD24" s="3"/>
+      <c r="AE24" s="3"/>
+      <c r="AF24" s="3"/>
+      <c r="AG24" s="3"/>
+      <c r="AH24" s="3"/>
+    </row>
+    <row r="25" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1</v>
       </c>
@@ -868,8 +2041,57 @@
       <c r="E25" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F25" s="5"/>
+      <c r="H25" s="6">
+        <v>1</v>
+      </c>
+      <c r="I25" s="6">
+        <v>20</v>
+      </c>
+      <c r="J25" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="K25" s="6">
+        <v>0.29959999999999998</v>
+      </c>
+      <c r="L25" s="6">
+        <v>0.67510000000000003</v>
+      </c>
+      <c r="M25" s="6">
+        <v>37.35</v>
+      </c>
+      <c r="N25" s="3"/>
+      <c r="O25" s="6">
+        <v>1</v>
+      </c>
+      <c r="P25" s="6">
+        <v>20</v>
+      </c>
+      <c r="Q25" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="R25" s="6">
+        <v>0.21179999999999999</v>
+      </c>
+      <c r="S25" s="6">
+        <v>0.57920000000000005</v>
+      </c>
+      <c r="T25" s="6">
+        <v>57.7</v>
+      </c>
+      <c r="Z25" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA25" s="3"/>
+      <c r="AB25" s="3"/>
+      <c r="AC25" s="3"/>
+      <c r="AD25" s="3"/>
+      <c r="AE25" s="3"/>
+      <c r="AF25" s="3"/>
+      <c r="AG25" s="3"/>
+      <c r="AH25" s="3"/>
+    </row>
+    <row r="26" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2</v>
       </c>
@@ -885,11 +2107,47 @@
       <c r="E26" t="s">
         <v>5</v>
       </c>
-      <c r="F26" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F26" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H26" s="6">
+        <v>1</v>
+      </c>
+      <c r="I26" s="6">
+        <v>20</v>
+      </c>
+      <c r="J26" s="6">
+        <v>1</v>
+      </c>
+      <c r="K26" s="6"/>
+      <c r="L26" s="6"/>
+      <c r="M26" s="6"/>
+      <c r="N26" s="3"/>
+      <c r="O26" s="6">
+        <v>1</v>
+      </c>
+      <c r="P26" s="6">
+        <v>20</v>
+      </c>
+      <c r="Q26" s="6">
+        <v>1</v>
+      </c>
+      <c r="R26" s="6"/>
+      <c r="S26" s="6"/>
+      <c r="T26" s="6"/>
+      <c r="Z26" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA26" s="3"/>
+      <c r="AB26" s="3"/>
+      <c r="AC26" s="3"/>
+      <c r="AD26" s="3"/>
+      <c r="AE26" s="3"/>
+      <c r="AF26" s="3"/>
+      <c r="AG26" s="3"/>
+      <c r="AH26" s="3"/>
+    </row>
+    <row r="27" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2</v>
       </c>
@@ -905,11 +2163,47 @@
       <c r="E27" t="s">
         <v>6</v>
       </c>
-      <c r="F27" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F27" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H27" s="6">
+        <v>1</v>
+      </c>
+      <c r="I27" s="6">
+        <v>20</v>
+      </c>
+      <c r="J27" s="6">
+        <v>2</v>
+      </c>
+      <c r="K27" s="6"/>
+      <c r="L27" s="6"/>
+      <c r="M27" s="6"/>
+      <c r="N27" s="3"/>
+      <c r="O27" s="6">
+        <v>1</v>
+      </c>
+      <c r="P27" s="6">
+        <v>20</v>
+      </c>
+      <c r="Q27" s="6">
+        <v>2</v>
+      </c>
+      <c r="R27" s="6"/>
+      <c r="S27" s="6"/>
+      <c r="T27" s="6"/>
+      <c r="Z27" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="AA27" s="3"/>
+      <c r="AB27" s="3"/>
+      <c r="AC27" s="3"/>
+      <c r="AD27" s="3"/>
+      <c r="AE27" s="3"/>
+      <c r="AF27" s="3"/>
+      <c r="AG27" s="3"/>
+      <c r="AH27" s="3"/>
+    </row>
+    <row r="28" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2</v>
       </c>
@@ -925,11 +2219,59 @@
       <c r="E28" t="s">
         <v>5</v>
       </c>
-      <c r="F28" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F28" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H28" s="6">
+        <v>2</v>
+      </c>
+      <c r="I28" s="6">
+        <v>5</v>
+      </c>
+      <c r="J28" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="K28" s="6">
+        <v>0.3735</v>
+      </c>
+      <c r="L28" s="6">
+        <v>0.78259999999999996</v>
+      </c>
+      <c r="M28" s="6">
+        <v>20.149999999999999</v>
+      </c>
+      <c r="N28" s="3"/>
+      <c r="O28" s="6">
+        <v>2</v>
+      </c>
+      <c r="P28" s="6">
+        <v>5</v>
+      </c>
+      <c r="Q28" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="R28" s="6">
+        <v>0.33689999999999998</v>
+      </c>
+      <c r="S28" s="6">
+        <v>0.77249999999999996</v>
+      </c>
+      <c r="T28" s="6">
+        <v>24.05</v>
+      </c>
+      <c r="Z28" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA28" s="3"/>
+      <c r="AB28" s="3"/>
+      <c r="AC28" s="3"/>
+      <c r="AD28" s="3"/>
+      <c r="AE28" s="3"/>
+      <c r="AF28" s="3"/>
+      <c r="AG28" s="3"/>
+      <c r="AH28" s="3"/>
+    </row>
+    <row r="29" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2</v>
       </c>
@@ -945,11 +2287,53 @@
       <c r="E29" t="s">
         <v>6</v>
       </c>
-      <c r="F29" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F29" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H29" s="6">
+        <v>2</v>
+      </c>
+      <c r="I29" s="6">
+        <v>5</v>
+      </c>
+      <c r="J29" s="6">
+        <v>1</v>
+      </c>
+      <c r="K29" s="6"/>
+      <c r="L29" s="6"/>
+      <c r="M29" s="6"/>
+      <c r="N29" s="3"/>
+      <c r="O29" s="6">
+        <v>2</v>
+      </c>
+      <c r="P29" s="6">
+        <v>5</v>
+      </c>
+      <c r="Q29" s="6">
+        <v>1</v>
+      </c>
+      <c r="R29" s="6">
+        <v>0</v>
+      </c>
+      <c r="S29" s="6">
+        <v>0</v>
+      </c>
+      <c r="T29" s="6">
+        <v>13</v>
+      </c>
+      <c r="Z29" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA29" s="3"/>
+      <c r="AB29" s="3"/>
+      <c r="AC29" s="3"/>
+      <c r="AD29" s="3"/>
+      <c r="AE29" s="3"/>
+      <c r="AF29" s="3"/>
+      <c r="AG29" s="3"/>
+      <c r="AH29" s="3"/>
+    </row>
+    <row r="30" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2</v>
       </c>
@@ -965,11 +2349,59 @@
       <c r="E30" t="s">
         <v>5</v>
       </c>
-      <c r="F30" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F30" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H30" s="6">
+        <v>2</v>
+      </c>
+      <c r="I30" s="6">
+        <v>10</v>
+      </c>
+      <c r="J30" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="K30" s="6">
+        <v>5.3100000000000001E-2</v>
+      </c>
+      <c r="L30" s="6">
+        <v>0.40389999999999998</v>
+      </c>
+      <c r="M30" s="6">
+        <v>236.2</v>
+      </c>
+      <c r="N30" s="3"/>
+      <c r="O30" s="6">
+        <v>2</v>
+      </c>
+      <c r="P30" s="6">
+        <v>10</v>
+      </c>
+      <c r="Q30" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="R30" s="6">
+        <v>0.26069999999999999</v>
+      </c>
+      <c r="S30" s="6">
+        <v>0.63680000000000003</v>
+      </c>
+      <c r="T30" s="6">
+        <v>37.549999999999997</v>
+      </c>
+      <c r="Z30" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA30" s="3"/>
+      <c r="AB30" s="3"/>
+      <c r="AC30" s="3"/>
+      <c r="AD30" s="3"/>
+      <c r="AE30" s="3"/>
+      <c r="AF30" s="3"/>
+      <c r="AG30" s="3"/>
+      <c r="AH30" s="3"/>
+    </row>
+    <row r="31" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2</v>
       </c>
@@ -985,11 +2417,36 @@
       <c r="E31" t="s">
         <v>6</v>
       </c>
-      <c r="F31" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F31" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H31" s="6">
+        <v>2</v>
+      </c>
+      <c r="I31" s="6">
+        <v>10</v>
+      </c>
+      <c r="J31" s="6">
+        <v>1</v>
+      </c>
+      <c r="K31" s="6"/>
+      <c r="L31" s="6"/>
+      <c r="M31" s="6"/>
+      <c r="N31" s="3"/>
+      <c r="O31" s="6">
+        <v>2</v>
+      </c>
+      <c r="P31" s="6">
+        <v>10</v>
+      </c>
+      <c r="Q31" s="6">
+        <v>1</v>
+      </c>
+      <c r="R31" s="6"/>
+      <c r="S31" s="6"/>
+      <c r="T31" s="6"/>
+    </row>
+    <row r="32" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2</v>
       </c>
@@ -1005,8 +2462,46 @@
       <c r="E32" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F32" s="5"/>
+      <c r="H32" s="6">
+        <v>2</v>
+      </c>
+      <c r="I32" s="6">
+        <v>20</v>
+      </c>
+      <c r="J32" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="K32" s="6">
+        <v>4.87E-2</v>
+      </c>
+      <c r="L32" s="6">
+        <v>0.43869999999999998</v>
+      </c>
+      <c r="M32" s="6">
+        <v>255.5</v>
+      </c>
+      <c r="N32" s="3"/>
+      <c r="O32" s="6">
+        <v>2</v>
+      </c>
+      <c r="P32" s="6">
+        <v>20</v>
+      </c>
+      <c r="Q32" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="R32" s="6">
+        <v>5.2400000000000002E-2</v>
+      </c>
+      <c r="S32" s="6">
+        <v>0.44650000000000001</v>
+      </c>
+      <c r="T32" s="6">
+        <v>235.1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2</v>
       </c>
@@ -1022,8 +2517,36 @@
       <c r="E33" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F33" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H33" s="6">
+        <v>2</v>
+      </c>
+      <c r="I33" s="6">
+        <v>20</v>
+      </c>
+      <c r="J33" s="6">
+        <v>1</v>
+      </c>
+      <c r="K33" s="6"/>
+      <c r="L33" s="6"/>
+      <c r="M33" s="6"/>
+      <c r="N33" s="3"/>
+      <c r="O33" s="6">
+        <v>2</v>
+      </c>
+      <c r="P33" s="6">
+        <v>20</v>
+      </c>
+      <c r="Q33" s="6">
+        <v>1</v>
+      </c>
+      <c r="R33" s="6"/>
+      <c r="S33" s="6"/>
+      <c r="T33" s="6"/>
+    </row>
+    <row r="34" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2</v>
       </c>
@@ -1039,11 +2562,36 @@
       <c r="E34" t="s">
         <v>5</v>
       </c>
-      <c r="F34" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F34" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H34" s="6">
+        <v>2</v>
+      </c>
+      <c r="I34" s="6">
+        <v>20</v>
+      </c>
+      <c r="J34" s="6">
+        <v>2</v>
+      </c>
+      <c r="K34" s="6"/>
+      <c r="L34" s="6"/>
+      <c r="M34" s="6"/>
+      <c r="N34" s="3"/>
+      <c r="O34" s="6">
+        <v>2</v>
+      </c>
+      <c r="P34" s="6">
+        <v>20</v>
+      </c>
+      <c r="Q34" s="6">
+        <v>2</v>
+      </c>
+      <c r="R34" s="6"/>
+      <c r="S34" s="6"/>
+      <c r="T34" s="6"/>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>2</v>
       </c>
@@ -1059,11 +2607,11 @@
       <c r="E35" t="s">
         <v>6</v>
       </c>
-      <c r="F35" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F35" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>2</v>
       </c>
@@ -1079,11 +2627,19 @@
       <c r="E36" t="s">
         <v>5</v>
       </c>
-      <c r="F36" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F36" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+      <c r="M36" s="2"/>
+    </row>
+    <row r="37" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2</v>
       </c>
@@ -1099,11 +2655,29 @@
       <c r="E37" t="s">
         <v>6</v>
       </c>
-      <c r="F37" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F37" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I37" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J37" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K37" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L37" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="M37" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2</v>
       </c>
@@ -1119,8 +2693,32 @@
       <c r="E38" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F38" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H38" s="3">
+        <v>1</v>
+      </c>
+      <c r="I38" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="J38" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="K38" s="3">
+        <v>0.1691</v>
+      </c>
+      <c r="L38" s="3">
+        <v>0.35709999999999997</v>
+      </c>
+      <c r="M38" s="3">
+        <v>34.799999999999997</v>
+      </c>
+      <c r="N38" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>2</v>
       </c>
@@ -1136,8 +2734,32 @@
       <c r="E39" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F39" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H39" s="3">
+        <v>1</v>
+      </c>
+      <c r="I39" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="J39" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="K39" s="3">
+        <v>0.24229999999999999</v>
+      </c>
+      <c r="L39" s="3">
+        <v>0.50880000000000003</v>
+      </c>
+      <c r="M39" s="3">
+        <v>32.25</v>
+      </c>
+      <c r="N39" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>2</v>
       </c>
@@ -1154,7 +2776,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>2</v>
       </c>
@@ -1171,7 +2793,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>2</v>
       </c>
@@ -1187,11 +2809,11 @@
       <c r="E42" t="s">
         <v>5</v>
       </c>
-      <c r="F42" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F42" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>2</v>
       </c>
@@ -1207,11 +2829,11 @@
       <c r="E43" t="s">
         <v>6</v>
       </c>
-      <c r="F43" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F43" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>2</v>
       </c>
@@ -1227,11 +2849,11 @@
       <c r="E44" t="s">
         <v>5</v>
       </c>
-      <c r="F44" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F44" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>2</v>
       </c>
@@ -1247,11 +2869,11 @@
       <c r="E45" t="s">
         <v>6</v>
       </c>
-      <c r="F45" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F45" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>2</v>
       </c>
@@ -1268,7 +2890,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>2</v>
       </c>
@@ -1285,7 +2907,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>2</v>
       </c>
@@ -1320,6 +2942,20 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="H36:M36"/>
+    <mergeCell ref="Z3:AC3"/>
+    <mergeCell ref="AE3:AH3"/>
+    <mergeCell ref="Z1:AH2"/>
+    <mergeCell ref="Z13:AC13"/>
+    <mergeCell ref="AE13:AH13"/>
+    <mergeCell ref="Z23:AC23"/>
+    <mergeCell ref="H3:M3"/>
+    <mergeCell ref="O3:T3"/>
+    <mergeCell ref="H19:M19"/>
+    <mergeCell ref="O19:T19"/>
+    <mergeCell ref="H1:T2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>